<commit_message>
update README and minot mapping adjustments
</commit_message>
<xml_diff>
--- a/ontology mapping.xlsx
+++ b/ontology mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\peter\dev\evaluation_bachelor_thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB221B37-E1C9-423C-900B-2898DD63A0A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AF3115-E637-4B59-A53C-54BEE2A7B217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{DA29BB5A-9ECC-4C74-A178-3B4DA92462C7}"/>
+    <workbookView xWindow="-69" yWindow="-69" windowWidth="33052" windowHeight="18052" xr2:uid="{DA29BB5A-9ECC-4C74-A178-3B4DA92462C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="162">
   <si>
     <t>Thing</t>
   </si>
@@ -523,6 +523,9 @@
   </si>
   <si>
     <t>governmental organization (took the more generic type instead of public body in wikidata)</t>
+  </si>
+  <si>
+    <t>P1320</t>
   </si>
 </sst>
 </file>
@@ -907,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36170524-7C4F-4E1D-93D7-1517FE78070A}">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1303,6 +1306,12 @@
       <c r="A41" t="s">
         <v>89</v>
       </c>
+      <c r="B41" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" t="s">
+        <v>54</v>
+      </c>
       <c r="D41" t="s">
         <v>90</v>
       </c>

</xml_diff>